<commit_message>
Adding Scenario 9 for customer default (collections) - Update README. - Update Excel sheet. - Add Scenario JSON & JSONL files.
</commit_message>
<xml_diff>
--- a/Data Exchange Schema - Scenarios.xlsx
+++ b/Data Exchange Schema - Scenarios.xlsx
@@ -12,6 +12,7 @@
     <sheet state="visible" name="Scenario 6" sheetId="7" r:id="rId10"/>
     <sheet state="visible" name="Scenario 7" sheetId="8" r:id="rId11"/>
     <sheet state="visible" name="Scenario 8" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="Scenario 9" sheetId="10" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="87">
   <si>
     <t>Summary</t>
   </si>
@@ -73,6 +74,12 @@
   </si>
   <si>
     <t>Scenario 8</t>
+  </si>
+  <si>
+    <t>Scenario 9</t>
+  </si>
+  <si>
+    <t>Transaction of €150 with 3 installments, with 2nd &amp; 3rd installment late, then written off (sent to collections)</t>
   </si>
   <si>
     <t>Effective Timestamp</t>
@@ -271,6 +278,12 @@
   </si>
   <si>
     <t>13.34 EUR</t>
+  </si>
+  <si>
+    <t>installmentWrittenOff</t>
+  </si>
+  <si>
+    <t>ConsumerDefault</t>
   </si>
 </sst>
 </file>
@@ -950,7 +963,7 @@
       <border/>
     </dxf>
   </dxfs>
-  <tableStyles count="8">
+  <tableStyles count="9">
     <tableStyle count="3" pivot="0" name="Scenario 1-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
@@ -991,11 +1004,20 @@
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="4" type="secondRowStripe"/>
     </tableStyle>
+    <tableStyle count="3" pivot="0" name="Scenario 9-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="4" type="secondRowStripe"/>
+    </tableStyle>
   </tableStyles>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1161,6 +1183,23 @@
     <tableColumn name="Additional Details" id="9"/>
   </tableColumns>
   <tableStyleInfo name="Scenario 8-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B4:J11" displayName="Table9" name="Table9" id="9">
+  <tableColumns count="9">
+    <tableColumn name="Effective Timestamp" id="1"/>
+    <tableColumn name="Type" id="2"/>
+    <tableColumn name="Order ID" id="3"/>
+    <tableColumn name="Installment ID" id="4"/>
+    <tableColumn name="Amount" id="5"/>
+    <tableColumn name="Transaction Type" id="6"/>
+    <tableColumn name="Due Timestamp" id="7"/>
+    <tableColumn name="Index" id="8"/>
+    <tableColumn name="Additional Details" id="9"/>
+  </tableColumns>
+  <tableStyleInfo name="Scenario 9-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -1450,8 +1489,307 @@
         <v>16</v>
       </c>
     </row>
+    <row r="16">
+      <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="23.13"/>
+    <col customWidth="1" min="2" max="2" width="24.13"/>
+    <col customWidth="1" min="3" max="3" width="23.13"/>
+    <col customWidth="1" min="4" max="4" width="14.75"/>
+    <col customWidth="1" min="5" max="5" width="19.0"/>
+    <col customWidth="1" min="6" max="6" width="11.38"/>
+    <col customWidth="1" min="7" max="7" width="23.13"/>
+    <col customWidth="1" min="8" max="8" width="17.5"/>
+    <col customWidth="1" min="9" max="9" width="9.5"/>
+    <col customWidth="1" min="10" max="10" width="21.75"/>
+    <col customWidth="1" min="11" max="26" width="23.13"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" s="88"/>
+    </row>
+    <row r="4">
+      <c r="B4" s="76" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="77" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="77" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="77" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="78" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="19">
+        <v>45691.0</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="79" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="79" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="79" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="80" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="69">
+        <v>45691.0</v>
+      </c>
+      <c r="C6" s="81" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="82" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="81" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="71">
+        <v>45691.0</v>
+      </c>
+      <c r="I6" s="82">
+        <v>0.0</v>
+      </c>
+      <c r="J6" s="83" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="19">
+        <v>45691.0</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="79" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="23">
+        <v>45721.0</v>
+      </c>
+      <c r="I7" s="79">
+        <v>1.0</v>
+      </c>
+      <c r="J7" s="80" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="69">
+        <v>45691.0</v>
+      </c>
+      <c r="C8" s="81" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="82" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="81" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="71">
+        <v>45751.0</v>
+      </c>
+      <c r="I8" s="82">
+        <v>2.0</v>
+      </c>
+      <c r="J8" s="83" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="19">
+        <v>45691.0</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="79" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="79" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="79" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="80" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="32">
+        <v>45901.0</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="82" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" s="82" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="K10" s="84"/>
+    </row>
+    <row r="11">
+      <c r="B11" s="39">
+        <v>45901.0</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="85" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="86" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="86" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="41" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" sqref="E5:E11">
+      <formula1>"installment-1,installment-2,installment-3"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="J5:J11">
+      <formula1>"-,ConsumerDefault"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="G5:G11">
+      <formula1>"PayIn3,-"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B5:B11">
+      <formula1>OR(NOT(ISERROR(DATEVALUE(B5))), AND(ISNUMBER(B5), LEFT(CELL("format", B5))="D"))</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="D5:D11">
+      <formula1>"order-1"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="C5:C11">
+      <formula1>"transactionCreated,installmentIssued,installmentPaid,refundIssued,installmentWrittenOff"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1504,31 +1842,31 @@
     </row>
     <row r="4">
       <c r="B4" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5">
@@ -1536,24 +1874,24 @@
         <v>45691.0</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6">
@@ -1561,19 +1899,19 @@
         <v>45691.0</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H6" s="17">
         <v>45691.0</v>
@@ -1582,7 +1920,7 @@
         <v>0.0</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7">
@@ -1590,19 +1928,19 @@
         <v>45691.0</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H7" s="23">
         <v>45721.0</v>
@@ -1611,7 +1949,7 @@
         <v>1.0</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8">
@@ -1619,19 +1957,19 @@
         <v>45691.0</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E8" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="16" t="s">
-        <v>34</v>
-      </c>
       <c r="G8" s="13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H8" s="17">
         <v>45751.0</v>
@@ -1640,7 +1978,7 @@
         <v>2.0</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9">
@@ -1648,28 +1986,28 @@
         <v>45691.0</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10">
@@ -1677,28 +2015,28 @@
         <v>45721.0</v>
       </c>
       <c r="C10" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>35</v>
-      </c>
       <c r="F10" s="16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11">
@@ -1706,28 +2044,28 @@
         <v>45751.0</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="29" t="s">
-        <v>34</v>
-      </c>
       <c r="G11" s="26" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H11" s="29" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I11" s="30" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1786,34 +2124,34 @@
     </row>
     <row r="4">
       <c r="B4" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5">
@@ -1821,27 +2159,27 @@
         <v>45691.0</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6">
@@ -1849,19 +2187,19 @@
         <v>45691.0</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F6" s="35" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G6" s="33" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H6" s="36">
         <v>45691.0</v>
@@ -1870,10 +2208,10 @@
         <v>0.0</v>
       </c>
       <c r="J6" s="37" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7">
@@ -1881,19 +2219,19 @@
         <v>45691.0</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H7" s="38">
         <v>45721.0</v>
@@ -1902,10 +2240,10 @@
         <v>1.0</v>
       </c>
       <c r="J7" s="31" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8">
@@ -1913,19 +2251,19 @@
         <v>45691.0</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E8" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="35" t="s">
-        <v>34</v>
-      </c>
       <c r="G8" s="33" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H8" s="36">
         <v>45751.0</v>
@@ -1934,10 +2272,10 @@
         <v>2.0</v>
       </c>
       <c r="J8" s="37" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9">
@@ -1945,31 +2283,31 @@
         <v>45691.0</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J9" s="31" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10">
@@ -1977,31 +2315,31 @@
         <v>45720.0</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F10" s="35" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G10" s="33" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H10" s="36">
         <v>45728.0</v>
       </c>
       <c r="I10" s="35" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J10" s="37" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11">
@@ -2009,31 +2347,31 @@
         <v>45720.0</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H11" s="38">
         <v>45758.0</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J11" s="31" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12">
@@ -2041,31 +2379,31 @@
         <v>45720.0</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E12" s="33" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F12" s="35" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G12" s="33" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H12" s="35" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I12" s="35" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J12" s="37" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13">
@@ -2073,31 +2411,31 @@
         <v>45728.0</v>
       </c>
       <c r="C13" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>35</v>
-      </c>
       <c r="F13" s="10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J13" s="31" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14">
@@ -2105,31 +2443,31 @@
         <v>45728.0</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E14" s="33" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F14" s="35" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G14" s="33" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H14" s="35" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I14" s="35" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J14" s="37" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15">
@@ -2137,31 +2475,31 @@
         <v>45758.0</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E15" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="40" t="s">
-        <v>34</v>
-      </c>
       <c r="G15" s="28" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H15" s="40" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I15" s="40" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J15" s="41" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2223,34 +2561,34 @@
     <row r="4">
       <c r="A4" s="42"/>
       <c r="B4" s="43" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" s="45" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F4" s="44" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G4" s="44" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H4" s="44" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I4" s="44" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J4" s="46" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K4" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L4" s="42"/>
       <c r="M4" s="42"/>
@@ -2272,27 +2610,27 @@
         <v>45691.0</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="49"/>
       <c r="F5" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="42" t="s">
         <v>28</v>
-      </c>
-      <c r="G5" s="49" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="42" t="s">
-        <v>26</v>
       </c>
       <c r="L5" s="42"/>
       <c r="M5" s="42"/>
@@ -2314,19 +2652,19 @@
         <v>45691.0</v>
       </c>
       <c r="C6" s="53" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F6" s="54" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G6" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H6" s="55">
         <v>45691.0</v>
@@ -2335,10 +2673,10 @@
         <v>0.0</v>
       </c>
       <c r="J6" s="57" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K6" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L6" s="42"/>
       <c r="M6" s="42"/>
@@ -2360,19 +2698,19 @@
         <v>45691.0</v>
       </c>
       <c r="C7" s="49" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F7" s="50" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G7" s="49" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H7" s="58">
         <v>45721.0</v>
@@ -2381,10 +2719,10 @@
         <v>1.0</v>
       </c>
       <c r="J7" s="51" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K7" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L7" s="42"/>
       <c r="M7" s="42"/>
@@ -2406,19 +2744,19 @@
         <v>45691.0</v>
       </c>
       <c r="C8" s="53" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E8" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="54" t="s">
-        <v>34</v>
-      </c>
       <c r="G8" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H8" s="55">
         <v>45751.0</v>
@@ -2427,10 +2765,10 @@
         <v>2.0</v>
       </c>
       <c r="J8" s="57" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K8" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L8" s="42"/>
       <c r="M8" s="42"/>
@@ -2452,31 +2790,31 @@
         <v>45691.0</v>
       </c>
       <c r="C9" s="49" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F9" s="50" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G9" s="49" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H9" s="50" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I9" s="50" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J9" s="51" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K9" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L9" s="42"/>
       <c r="M9" s="42"/>
@@ -2498,31 +2836,31 @@
         <v>45724.0</v>
       </c>
       <c r="C10" s="60" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G10" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H10" s="55">
         <v>45721.0</v>
       </c>
       <c r="I10" s="54" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J10" s="57" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="K10" s="61" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="L10" s="42"/>
       <c r="M10" s="42"/>
@@ -2544,31 +2882,31 @@
         <v>45727.0</v>
       </c>
       <c r="C11" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>35</v>
-      </c>
       <c r="F11" s="50" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G11" s="49" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H11" s="50" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I11" s="50" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J11" s="51" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K11" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L11" s="42"/>
       <c r="M11" s="42"/>
@@ -2590,31 +2928,31 @@
         <v>45727.0</v>
       </c>
       <c r="C12" s="53" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F12" s="54" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G12" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H12" s="54" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I12" s="54" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J12" s="57" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K12" s="61" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="L12" s="42"/>
       <c r="M12" s="42"/>
@@ -2636,31 +2974,31 @@
         <v>45751.0</v>
       </c>
       <c r="C13" s="63" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E13" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="64" t="s">
-        <v>34</v>
-      </c>
       <c r="G13" s="63" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H13" s="64" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I13" s="64" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J13" s="65" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K13" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L13" s="42"/>
       <c r="M13" s="42"/>
@@ -2735,34 +3073,34 @@
     <row r="4">
       <c r="A4" s="42"/>
       <c r="B4" s="43" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" s="45" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F4" s="44" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G4" s="44" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H4" s="44" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I4" s="44" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J4" s="46" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K4" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L4" s="42"/>
       <c r="M4" s="42"/>
@@ -2784,27 +3122,27 @@
         <v>45691.0</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="49"/>
       <c r="F5" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="42" t="s">
         <v>28</v>
-      </c>
-      <c r="G5" s="49" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="42" t="s">
-        <v>26</v>
       </c>
       <c r="L5" s="42"/>
       <c r="M5" s="42"/>
@@ -2826,19 +3164,19 @@
         <v>45691.0</v>
       </c>
       <c r="C6" s="53" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F6" s="54" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G6" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H6" s="55">
         <v>45691.0</v>
@@ -2847,10 +3185,10 @@
         <v>0.0</v>
       </c>
       <c r="J6" s="57" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K6" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L6" s="42"/>
       <c r="M6" s="42"/>
@@ -2872,19 +3210,19 @@
         <v>45691.0</v>
       </c>
       <c r="C7" s="49" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F7" s="50" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G7" s="49" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H7" s="58">
         <v>45721.0</v>
@@ -2893,10 +3231,10 @@
         <v>1.0</v>
       </c>
       <c r="J7" s="51" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K7" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L7" s="42"/>
       <c r="M7" s="42"/>
@@ -2918,19 +3256,19 @@
         <v>45691.0</v>
       </c>
       <c r="C8" s="53" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E8" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="54" t="s">
-        <v>34</v>
-      </c>
       <c r="G8" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H8" s="55">
         <v>45751.0</v>
@@ -2939,10 +3277,10 @@
         <v>2.0</v>
       </c>
       <c r="J8" s="57" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K8" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L8" s="42"/>
       <c r="M8" s="42"/>
@@ -2964,31 +3302,31 @@
         <v>45691.0</v>
       </c>
       <c r="C9" s="49" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F9" s="50" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G9" s="49" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H9" s="50" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I9" s="50" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J9" s="51" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K9" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L9" s="42"/>
       <c r="M9" s="42"/>
@@ -3010,23 +3348,23 @@
         <v>45693.0</v>
       </c>
       <c r="C10" s="60" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D10" s="53"/>
       <c r="E10" s="53"/>
       <c r="F10" s="66" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G10" s="53"/>
       <c r="H10" s="54" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I10" s="54" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J10" s="57"/>
       <c r="K10" s="61" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="L10" s="42"/>
       <c r="M10" s="42"/>
@@ -3048,31 +3386,31 @@
         <v>45693.0</v>
       </c>
       <c r="C11" s="49" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F11" s="50" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G11" s="49" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H11" s="67" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I11" s="50" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J11" s="51" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K11" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L11" s="42"/>
       <c r="M11" s="42"/>
@@ -3094,28 +3432,28 @@
         <v>45693.0</v>
       </c>
       <c r="C12" s="53" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F12" s="54" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G12" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H12" s="54" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I12" s="54" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J12" s="57" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L12" s="42"/>
       <c r="M12" s="42"/>
@@ -3137,31 +3475,31 @@
         <v>45721.0</v>
       </c>
       <c r="C13" s="63" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="28" t="s">
-        <v>35</v>
-      </c>
       <c r="F13" s="64" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G13" s="63" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H13" s="64" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I13" s="64" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J13" s="65" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K13" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L13" s="42"/>
       <c r="M13" s="42"/>
@@ -3233,28 +3571,28 @@
     </row>
     <row r="4">
       <c r="B4" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5">
@@ -3262,24 +3600,24 @@
         <v>45691.0</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6">
@@ -3287,19 +3625,19 @@
         <v>45691.0</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F6" s="68" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H6" s="17">
         <v>45721.0</v>
@@ -3308,7 +3646,7 @@
         <v>0.0</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7">
@@ -3316,25 +3654,25 @@
         <v>45721.0</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F7" s="40" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G7" s="26" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I7" s="30" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -3393,28 +3731,28 @@
     </row>
     <row r="4">
       <c r="B4" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5">
@@ -3422,21 +3760,21 @@
         <v>45691.0</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="22" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6">
@@ -3444,19 +3782,19 @@
         <v>45692.0</v>
       </c>
       <c r="C6" s="70" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F6" s="35" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G6" s="70" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H6" s="71">
         <v>45692.0</v>
@@ -3465,7 +3803,7 @@
         <v>0.0</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7">
@@ -3473,19 +3811,19 @@
         <v>45692.0</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H7" s="23">
         <v>45722.0</v>
@@ -3494,7 +3832,7 @@
         <v>1.0</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8">
@@ -3502,19 +3840,19 @@
         <v>45692.0</v>
       </c>
       <c r="C8" s="70" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F8" s="35" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G8" s="70" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H8" s="71">
         <v>45752.0</v>
@@ -3528,28 +3866,28 @@
         <v>45692.0</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10">
@@ -3557,19 +3895,19 @@
         <v>45696.0</v>
       </c>
       <c r="C10" s="70" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F10" s="35" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G10" s="70" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H10" s="71">
         <v>45696.0</v>
@@ -3578,7 +3916,7 @@
         <v>0.0</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11">
@@ -3586,19 +3924,19 @@
         <v>45696.0</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H11" s="23">
         <v>45726.0</v>
@@ -3607,7 +3945,7 @@
         <v>1.0</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12">
@@ -3615,19 +3953,19 @@
         <v>45696.0</v>
       </c>
       <c r="C12" s="70" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E12" s="33" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F12" s="35" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G12" s="70" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H12" s="71">
         <v>45756.0</v>
@@ -3641,28 +3979,28 @@
         <v>45696.0</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14">
@@ -3670,25 +4008,25 @@
         <v>45722.0</v>
       </c>
       <c r="C14" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="33" t="s">
-        <v>35</v>
-      </c>
       <c r="F14" s="35" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G14" s="70" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H14" s="73" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I14" s="72" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15">
@@ -3696,25 +4034,25 @@
         <v>45726.0</v>
       </c>
       <c r="C15" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>35</v>
-      </c>
       <c r="F15" s="10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H15" s="22" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16">
@@ -3722,25 +4060,25 @@
         <v>45752.0</v>
       </c>
       <c r="C16" s="70" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E16" s="33" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F16" s="35" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G16" s="70" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H16" s="73" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I16" s="72" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17">
@@ -3748,25 +4086,25 @@
         <v>45756.0</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F17" s="40" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G17" s="26" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H17" s="29" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I17" s="74" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -3828,36 +4166,36 @@
     </row>
     <row r="2">
       <c r="C2" s="75" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="76" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C4" s="77" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F4" s="77" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G4" s="77" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H4" s="77" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I4" s="77" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J4" s="78" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
@@ -3865,24 +4203,24 @@
         <v>45691.0</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="79" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H5" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I5" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J5" s="80" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6">
@@ -3890,19 +4228,19 @@
         <v>45691.0</v>
       </c>
       <c r="C6" s="81" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F6" s="82" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G6" s="81" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H6" s="71">
         <v>45691.0</v>
@@ -3911,7 +4249,7 @@
         <v>0.0</v>
       </c>
       <c r="J6" s="83" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7">
@@ -3919,19 +4257,19 @@
         <v>45691.0</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F7" s="79" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H7" s="23">
         <v>45721.0</v>
@@ -3940,7 +4278,7 @@
         <v>1.0</v>
       </c>
       <c r="J7" s="80" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8">
@@ -3948,19 +4286,19 @@
         <v>45691.0</v>
       </c>
       <c r="C8" s="81" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E8" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="82" t="s">
-        <v>34</v>
-      </c>
       <c r="G8" s="81" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H8" s="71">
         <v>45751.0</v>
@@ -3969,7 +4307,7 @@
         <v>2.0</v>
       </c>
       <c r="J8" s="83" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9">
@@ -3977,28 +4315,28 @@
         <v>45691.0</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F9" s="79" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H9" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I9" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J9" s="80" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10">
@@ -4006,24 +4344,24 @@
         <v>45693.0</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D10" s="81"/>
       <c r="E10" s="81"/>
       <c r="F10" s="35" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G10" s="33" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H10" s="82" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I10" s="82" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J10" s="37" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K10" s="84"/>
     </row>
@@ -4032,28 +4370,28 @@
         <v>45693.0</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F11" s="79" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H11" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I11" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J11" s="80" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12">
@@ -4061,28 +4399,28 @@
         <v>45693.0</v>
       </c>
       <c r="C12" s="81" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E12" s="33" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F12" s="35" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G12" s="81" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H12" s="82" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I12" s="82" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J12" s="83" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13">
@@ -4090,31 +4428,31 @@
         <v>45691.0</v>
       </c>
       <c r="C13" s="85" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F13" s="40" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G13" s="85" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H13" s="86" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I13" s="86" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J13" s="87" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25">
@@ -4187,36 +4525,36 @@
     </row>
     <row r="2">
       <c r="C2" s="88" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="76" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C4" s="77" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F4" s="77" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G4" s="77" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H4" s="77" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I4" s="77" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J4" s="78" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
@@ -4224,24 +4562,24 @@
         <v>45691.0</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="79" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H5" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I5" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J5" s="80" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6">
@@ -4249,19 +4587,19 @@
         <v>45691.0</v>
       </c>
       <c r="C6" s="81" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F6" s="82" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G6" s="81" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H6" s="71">
         <v>45691.0</v>
@@ -4270,7 +4608,7 @@
         <v>0.0</v>
       </c>
       <c r="J6" s="83" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7">
@@ -4278,19 +4616,19 @@
         <v>45691.0</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F7" s="79" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H7" s="23">
         <v>45721.0</v>
@@ -4299,7 +4637,7 @@
         <v>1.0</v>
       </c>
       <c r="J7" s="80" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8">
@@ -4307,19 +4645,19 @@
         <v>45691.0</v>
       </c>
       <c r="C8" s="81" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E8" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="82" t="s">
-        <v>34</v>
-      </c>
       <c r="G8" s="81" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H8" s="71">
         <v>45751.0</v>
@@ -4328,7 +4666,7 @@
         <v>2.0</v>
       </c>
       <c r="J8" s="83" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9">
@@ -4336,28 +4674,28 @@
         <v>45691.0</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F9" s="79" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H9" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I9" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J9" s="80" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10">
@@ -4365,24 +4703,24 @@
         <v>45693.0</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D10" s="81"/>
       <c r="E10" s="81"/>
       <c r="F10" s="35" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G10" s="33" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H10" s="82" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I10" s="82" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J10" s="37" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K10" s="84"/>
     </row>
@@ -4391,31 +4729,31 @@
         <v>45691.0</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H11" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I11" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J11" s="80" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12">
@@ -4423,28 +4761,28 @@
         <v>45693.0</v>
       </c>
       <c r="C12" s="81" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E12" s="33" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F12" s="35" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G12" s="81" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H12" s="82" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I12" s="82" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J12" s="83" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13">
@@ -4452,28 +4790,28 @@
         <v>45693.0</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H13" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I13" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J13" s="80" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14">
@@ -4481,28 +4819,28 @@
         <v>45721.0</v>
       </c>
       <c r="C14" s="81" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="33" t="s">
-        <v>35</v>
-      </c>
       <c r="F14" s="35" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G14" s="81" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H14" s="82" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I14" s="82" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J14" s="83" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15">
@@ -4510,28 +4848,28 @@
         <v>45751.0</v>
       </c>
       <c r="C15" s="90" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D15" s="91" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F15" s="92" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G15" s="93" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H15" s="94" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I15" s="94" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J15" s="95" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K15" s="96"/>
     </row>

</xml_diff>

<commit_message>
Adding Scenario 9 for customer default (collections) (#2)
- Update README.
- Update Excel sheet.
- Add Scenario JSON & JSONL files.
</commit_message>
<xml_diff>
--- a/Data Exchange Schema - Scenarios.xlsx
+++ b/Data Exchange Schema - Scenarios.xlsx
@@ -12,6 +12,7 @@
     <sheet state="visible" name="Scenario 6" sheetId="7" r:id="rId10"/>
     <sheet state="visible" name="Scenario 7" sheetId="8" r:id="rId11"/>
     <sheet state="visible" name="Scenario 8" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="Scenario 9" sheetId="10" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="87">
   <si>
     <t>Summary</t>
   </si>
@@ -73,6 +74,12 @@
   </si>
   <si>
     <t>Scenario 8</t>
+  </si>
+  <si>
+    <t>Scenario 9</t>
+  </si>
+  <si>
+    <t>Transaction of €150 with 3 installments, with 2nd &amp; 3rd installment late, then written off (sent to collections)</t>
   </si>
   <si>
     <t>Effective Timestamp</t>
@@ -271,6 +278,12 @@
   </si>
   <si>
     <t>13.34 EUR</t>
+  </si>
+  <si>
+    <t>installmentWrittenOff</t>
+  </si>
+  <si>
+    <t>ConsumerDefault</t>
   </si>
 </sst>
 </file>
@@ -950,7 +963,7 @@
       <border/>
     </dxf>
   </dxfs>
-  <tableStyles count="8">
+  <tableStyles count="9">
     <tableStyle count="3" pivot="0" name="Scenario 1-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
@@ -991,11 +1004,20 @@
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="4" type="secondRowStripe"/>
     </tableStyle>
+    <tableStyle count="3" pivot="0" name="Scenario 9-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="4" type="secondRowStripe"/>
+    </tableStyle>
   </tableStyles>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1161,6 +1183,23 @@
     <tableColumn name="Additional Details" id="9"/>
   </tableColumns>
   <tableStyleInfo name="Scenario 8-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B4:J11" displayName="Table9" name="Table9" id="9">
+  <tableColumns count="9">
+    <tableColumn name="Effective Timestamp" id="1"/>
+    <tableColumn name="Type" id="2"/>
+    <tableColumn name="Order ID" id="3"/>
+    <tableColumn name="Installment ID" id="4"/>
+    <tableColumn name="Amount" id="5"/>
+    <tableColumn name="Transaction Type" id="6"/>
+    <tableColumn name="Due Timestamp" id="7"/>
+    <tableColumn name="Index" id="8"/>
+    <tableColumn name="Additional Details" id="9"/>
+  </tableColumns>
+  <tableStyleInfo name="Scenario 9-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -1450,8 +1489,307 @@
         <v>16</v>
       </c>
     </row>
+    <row r="16">
+      <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="23.13"/>
+    <col customWidth="1" min="2" max="2" width="24.13"/>
+    <col customWidth="1" min="3" max="3" width="23.13"/>
+    <col customWidth="1" min="4" max="4" width="14.75"/>
+    <col customWidth="1" min="5" max="5" width="19.0"/>
+    <col customWidth="1" min="6" max="6" width="11.38"/>
+    <col customWidth="1" min="7" max="7" width="23.13"/>
+    <col customWidth="1" min="8" max="8" width="17.5"/>
+    <col customWidth="1" min="9" max="9" width="9.5"/>
+    <col customWidth="1" min="10" max="10" width="21.75"/>
+    <col customWidth="1" min="11" max="26" width="23.13"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" s="88"/>
+    </row>
+    <row r="4">
+      <c r="B4" s="76" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="77" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="77" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="77" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="78" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="19">
+        <v>45691.0</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="79" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="79" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="79" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="80" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="69">
+        <v>45691.0</v>
+      </c>
+      <c r="C6" s="81" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="82" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="81" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="71">
+        <v>45691.0</v>
+      </c>
+      <c r="I6" s="82">
+        <v>0.0</v>
+      </c>
+      <c r="J6" s="83" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="19">
+        <v>45691.0</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="79" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="23">
+        <v>45721.0</v>
+      </c>
+      <c r="I7" s="79">
+        <v>1.0</v>
+      </c>
+      <c r="J7" s="80" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="69">
+        <v>45691.0</v>
+      </c>
+      <c r="C8" s="81" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="82" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="81" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="71">
+        <v>45751.0</v>
+      </c>
+      <c r="I8" s="82">
+        <v>2.0</v>
+      </c>
+      <c r="J8" s="83" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="19">
+        <v>45691.0</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="79" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="79" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="79" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="80" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="32">
+        <v>45901.0</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="82" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" s="82" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="K10" s="84"/>
+    </row>
+    <row r="11">
+      <c r="B11" s="39">
+        <v>45901.0</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="85" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="86" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="86" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="41" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" sqref="E5:E11">
+      <formula1>"installment-1,installment-2,installment-3"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="J5:J11">
+      <formula1>"-,ConsumerDefault"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="G5:G11">
+      <formula1>"PayIn3,-"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B5:B11">
+      <formula1>OR(NOT(ISERROR(DATEVALUE(B5))), AND(ISNUMBER(B5), LEFT(CELL("format", B5))="D"))</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="D5:D11">
+      <formula1>"order-1"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="C5:C11">
+      <formula1>"transactionCreated,installmentIssued,installmentPaid,refundIssued,installmentWrittenOff"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1504,31 +1842,31 @@
     </row>
     <row r="4">
       <c r="B4" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5">
@@ -1536,24 +1874,24 @@
         <v>45691.0</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6">
@@ -1561,19 +1899,19 @@
         <v>45691.0</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H6" s="17">
         <v>45691.0</v>
@@ -1582,7 +1920,7 @@
         <v>0.0</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7">
@@ -1590,19 +1928,19 @@
         <v>45691.0</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H7" s="23">
         <v>45721.0</v>
@@ -1611,7 +1949,7 @@
         <v>1.0</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8">
@@ -1619,19 +1957,19 @@
         <v>45691.0</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E8" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="16" t="s">
-        <v>34</v>
-      </c>
       <c r="G8" s="13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H8" s="17">
         <v>45751.0</v>
@@ -1640,7 +1978,7 @@
         <v>2.0</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9">
@@ -1648,28 +1986,28 @@
         <v>45691.0</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10">
@@ -1677,28 +2015,28 @@
         <v>45721.0</v>
       </c>
       <c r="C10" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>35</v>
-      </c>
       <c r="F10" s="16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11">
@@ -1706,28 +2044,28 @@
         <v>45751.0</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="29" t="s">
-        <v>34</v>
-      </c>
       <c r="G11" s="26" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H11" s="29" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I11" s="30" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1786,34 +2124,34 @@
     </row>
     <row r="4">
       <c r="B4" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5">
@@ -1821,27 +2159,27 @@
         <v>45691.0</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6">
@@ -1849,19 +2187,19 @@
         <v>45691.0</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F6" s="35" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G6" s="33" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H6" s="36">
         <v>45691.0</v>
@@ -1870,10 +2208,10 @@
         <v>0.0</v>
       </c>
       <c r="J6" s="37" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7">
@@ -1881,19 +2219,19 @@
         <v>45691.0</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H7" s="38">
         <v>45721.0</v>
@@ -1902,10 +2240,10 @@
         <v>1.0</v>
       </c>
       <c r="J7" s="31" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8">
@@ -1913,19 +2251,19 @@
         <v>45691.0</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E8" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="35" t="s">
-        <v>34</v>
-      </c>
       <c r="G8" s="33" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H8" s="36">
         <v>45751.0</v>
@@ -1934,10 +2272,10 @@
         <v>2.0</v>
       </c>
       <c r="J8" s="37" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9">
@@ -1945,31 +2283,31 @@
         <v>45691.0</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J9" s="31" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10">
@@ -1977,31 +2315,31 @@
         <v>45720.0</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F10" s="35" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G10" s="33" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H10" s="36">
         <v>45728.0</v>
       </c>
       <c r="I10" s="35" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J10" s="37" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11">
@@ -2009,31 +2347,31 @@
         <v>45720.0</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H11" s="38">
         <v>45758.0</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J11" s="31" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12">
@@ -2041,31 +2379,31 @@
         <v>45720.0</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E12" s="33" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F12" s="35" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G12" s="33" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H12" s="35" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I12" s="35" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J12" s="37" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13">
@@ -2073,31 +2411,31 @@
         <v>45728.0</v>
       </c>
       <c r="C13" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>35</v>
-      </c>
       <c r="F13" s="10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J13" s="31" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14">
@@ -2105,31 +2443,31 @@
         <v>45728.0</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E14" s="33" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F14" s="35" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G14" s="33" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H14" s="35" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I14" s="35" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J14" s="37" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15">
@@ -2137,31 +2475,31 @@
         <v>45758.0</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E15" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="40" t="s">
-        <v>34</v>
-      </c>
       <c r="G15" s="28" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H15" s="40" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I15" s="40" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J15" s="41" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2223,34 +2561,34 @@
     <row r="4">
       <c r="A4" s="42"/>
       <c r="B4" s="43" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" s="45" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F4" s="44" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G4" s="44" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H4" s="44" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I4" s="44" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J4" s="46" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K4" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L4" s="42"/>
       <c r="M4" s="42"/>
@@ -2272,27 +2610,27 @@
         <v>45691.0</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="49"/>
       <c r="F5" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="42" t="s">
         <v>28</v>
-      </c>
-      <c r="G5" s="49" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="42" t="s">
-        <v>26</v>
       </c>
       <c r="L5" s="42"/>
       <c r="M5" s="42"/>
@@ -2314,19 +2652,19 @@
         <v>45691.0</v>
       </c>
       <c r="C6" s="53" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F6" s="54" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G6" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H6" s="55">
         <v>45691.0</v>
@@ -2335,10 +2673,10 @@
         <v>0.0</v>
       </c>
       <c r="J6" s="57" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K6" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L6" s="42"/>
       <c r="M6" s="42"/>
@@ -2360,19 +2698,19 @@
         <v>45691.0</v>
       </c>
       <c r="C7" s="49" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F7" s="50" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G7" s="49" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H7" s="58">
         <v>45721.0</v>
@@ -2381,10 +2719,10 @@
         <v>1.0</v>
       </c>
       <c r="J7" s="51" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K7" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L7" s="42"/>
       <c r="M7" s="42"/>
@@ -2406,19 +2744,19 @@
         <v>45691.0</v>
       </c>
       <c r="C8" s="53" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E8" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="54" t="s">
-        <v>34</v>
-      </c>
       <c r="G8" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H8" s="55">
         <v>45751.0</v>
@@ -2427,10 +2765,10 @@
         <v>2.0</v>
       </c>
       <c r="J8" s="57" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K8" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L8" s="42"/>
       <c r="M8" s="42"/>
@@ -2452,31 +2790,31 @@
         <v>45691.0</v>
       </c>
       <c r="C9" s="49" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F9" s="50" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G9" s="49" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H9" s="50" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I9" s="50" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J9" s="51" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K9" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L9" s="42"/>
       <c r="M9" s="42"/>
@@ -2498,31 +2836,31 @@
         <v>45724.0</v>
       </c>
       <c r="C10" s="60" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G10" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H10" s="55">
         <v>45721.0</v>
       </c>
       <c r="I10" s="54" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J10" s="57" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="K10" s="61" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="L10" s="42"/>
       <c r="M10" s="42"/>
@@ -2544,31 +2882,31 @@
         <v>45727.0</v>
       </c>
       <c r="C11" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>35</v>
-      </c>
       <c r="F11" s="50" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G11" s="49" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H11" s="50" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I11" s="50" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J11" s="51" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K11" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L11" s="42"/>
       <c r="M11" s="42"/>
@@ -2590,31 +2928,31 @@
         <v>45727.0</v>
       </c>
       <c r="C12" s="53" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F12" s="54" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G12" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H12" s="54" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I12" s="54" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J12" s="57" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K12" s="61" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="L12" s="42"/>
       <c r="M12" s="42"/>
@@ -2636,31 +2974,31 @@
         <v>45751.0</v>
       </c>
       <c r="C13" s="63" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E13" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="64" t="s">
-        <v>34</v>
-      </c>
       <c r="G13" s="63" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H13" s="64" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I13" s="64" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J13" s="65" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K13" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L13" s="42"/>
       <c r="M13" s="42"/>
@@ -2735,34 +3073,34 @@
     <row r="4">
       <c r="A4" s="42"/>
       <c r="B4" s="43" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" s="45" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F4" s="44" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G4" s="44" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H4" s="44" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I4" s="44" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J4" s="46" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K4" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L4" s="42"/>
       <c r="M4" s="42"/>
@@ -2784,27 +3122,27 @@
         <v>45691.0</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="49"/>
       <c r="F5" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="42" t="s">
         <v>28</v>
-      </c>
-      <c r="G5" s="49" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="42" t="s">
-        <v>26</v>
       </c>
       <c r="L5" s="42"/>
       <c r="M5" s="42"/>
@@ -2826,19 +3164,19 @@
         <v>45691.0</v>
       </c>
       <c r="C6" s="53" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F6" s="54" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G6" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H6" s="55">
         <v>45691.0</v>
@@ -2847,10 +3185,10 @@
         <v>0.0</v>
       </c>
       <c r="J6" s="57" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K6" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L6" s="42"/>
       <c r="M6" s="42"/>
@@ -2872,19 +3210,19 @@
         <v>45691.0</v>
       </c>
       <c r="C7" s="49" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F7" s="50" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G7" s="49" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H7" s="58">
         <v>45721.0</v>
@@ -2893,10 +3231,10 @@
         <v>1.0</v>
       </c>
       <c r="J7" s="51" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K7" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L7" s="42"/>
       <c r="M7" s="42"/>
@@ -2918,19 +3256,19 @@
         <v>45691.0</v>
       </c>
       <c r="C8" s="53" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E8" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="54" t="s">
-        <v>34</v>
-      </c>
       <c r="G8" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H8" s="55">
         <v>45751.0</v>
@@ -2939,10 +3277,10 @@
         <v>2.0</v>
       </c>
       <c r="J8" s="57" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K8" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L8" s="42"/>
       <c r="M8" s="42"/>
@@ -2964,31 +3302,31 @@
         <v>45691.0</v>
       </c>
       <c r="C9" s="49" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F9" s="50" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G9" s="49" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H9" s="50" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I9" s="50" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J9" s="51" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K9" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L9" s="42"/>
       <c r="M9" s="42"/>
@@ -3010,23 +3348,23 @@
         <v>45693.0</v>
       </c>
       <c r="C10" s="60" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D10" s="53"/>
       <c r="E10" s="53"/>
       <c r="F10" s="66" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G10" s="53"/>
       <c r="H10" s="54" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I10" s="54" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J10" s="57"/>
       <c r="K10" s="61" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="L10" s="42"/>
       <c r="M10" s="42"/>
@@ -3048,31 +3386,31 @@
         <v>45693.0</v>
       </c>
       <c r="C11" s="49" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F11" s="50" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G11" s="49" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H11" s="67" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I11" s="50" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J11" s="51" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K11" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L11" s="42"/>
       <c r="M11" s="42"/>
@@ -3094,28 +3432,28 @@
         <v>45693.0</v>
       </c>
       <c r="C12" s="53" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F12" s="54" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G12" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H12" s="54" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I12" s="54" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J12" s="57" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L12" s="42"/>
       <c r="M12" s="42"/>
@@ -3137,31 +3475,31 @@
         <v>45721.0</v>
       </c>
       <c r="C13" s="63" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="28" t="s">
-        <v>35</v>
-      </c>
       <c r="F13" s="64" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G13" s="63" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H13" s="64" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I13" s="64" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J13" s="65" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K13" s="42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L13" s="42"/>
       <c r="M13" s="42"/>
@@ -3233,28 +3571,28 @@
     </row>
     <row r="4">
       <c r="B4" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5">
@@ -3262,24 +3600,24 @@
         <v>45691.0</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6">
@@ -3287,19 +3625,19 @@
         <v>45691.0</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F6" s="68" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H6" s="17">
         <v>45721.0</v>
@@ -3308,7 +3646,7 @@
         <v>0.0</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7">
@@ -3316,25 +3654,25 @@
         <v>45721.0</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F7" s="40" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G7" s="26" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I7" s="30" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -3393,28 +3731,28 @@
     </row>
     <row r="4">
       <c r="B4" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5">
@@ -3422,21 +3760,21 @@
         <v>45691.0</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="22" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6">
@@ -3444,19 +3782,19 @@
         <v>45692.0</v>
       </c>
       <c r="C6" s="70" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F6" s="35" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G6" s="70" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H6" s="71">
         <v>45692.0</v>
@@ -3465,7 +3803,7 @@
         <v>0.0</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7">
@@ -3473,19 +3811,19 @@
         <v>45692.0</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H7" s="23">
         <v>45722.0</v>
@@ -3494,7 +3832,7 @@
         <v>1.0</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8">
@@ -3502,19 +3840,19 @@
         <v>45692.0</v>
       </c>
       <c r="C8" s="70" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F8" s="35" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G8" s="70" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H8" s="71">
         <v>45752.0</v>
@@ -3528,28 +3866,28 @@
         <v>45692.0</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10">
@@ -3557,19 +3895,19 @@
         <v>45696.0</v>
       </c>
       <c r="C10" s="70" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F10" s="35" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G10" s="70" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H10" s="71">
         <v>45696.0</v>
@@ -3578,7 +3916,7 @@
         <v>0.0</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11">
@@ -3586,19 +3924,19 @@
         <v>45696.0</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H11" s="23">
         <v>45726.0</v>
@@ -3607,7 +3945,7 @@
         <v>1.0</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12">
@@ -3615,19 +3953,19 @@
         <v>45696.0</v>
       </c>
       <c r="C12" s="70" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E12" s="33" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F12" s="35" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G12" s="70" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H12" s="71">
         <v>45756.0</v>
@@ -3641,28 +3979,28 @@
         <v>45696.0</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14">
@@ -3670,25 +4008,25 @@
         <v>45722.0</v>
       </c>
       <c r="C14" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="33" t="s">
-        <v>35</v>
-      </c>
       <c r="F14" s="35" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G14" s="70" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H14" s="73" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I14" s="72" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15">
@@ -3696,25 +4034,25 @@
         <v>45726.0</v>
       </c>
       <c r="C15" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>35</v>
-      </c>
       <c r="F15" s="10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H15" s="22" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16">
@@ -3722,25 +4060,25 @@
         <v>45752.0</v>
       </c>
       <c r="C16" s="70" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E16" s="33" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F16" s="35" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G16" s="70" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H16" s="73" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I16" s="72" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17">
@@ -3748,25 +4086,25 @@
         <v>45756.0</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F17" s="40" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G17" s="26" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H17" s="29" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I17" s="74" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -3828,36 +4166,36 @@
     </row>
     <row r="2">
       <c r="C2" s="75" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="76" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C4" s="77" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F4" s="77" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G4" s="77" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H4" s="77" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I4" s="77" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J4" s="78" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
@@ -3865,24 +4203,24 @@
         <v>45691.0</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="79" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H5" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I5" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J5" s="80" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6">
@@ -3890,19 +4228,19 @@
         <v>45691.0</v>
       </c>
       <c r="C6" s="81" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F6" s="82" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G6" s="81" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H6" s="71">
         <v>45691.0</v>
@@ -3911,7 +4249,7 @@
         <v>0.0</v>
       </c>
       <c r="J6" s="83" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7">
@@ -3919,19 +4257,19 @@
         <v>45691.0</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F7" s="79" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H7" s="23">
         <v>45721.0</v>
@@ -3940,7 +4278,7 @@
         <v>1.0</v>
       </c>
       <c r="J7" s="80" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8">
@@ -3948,19 +4286,19 @@
         <v>45691.0</v>
       </c>
       <c r="C8" s="81" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E8" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="82" t="s">
-        <v>34</v>
-      </c>
       <c r="G8" s="81" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H8" s="71">
         <v>45751.0</v>
@@ -3969,7 +4307,7 @@
         <v>2.0</v>
       </c>
       <c r="J8" s="83" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9">
@@ -3977,28 +4315,28 @@
         <v>45691.0</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F9" s="79" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H9" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I9" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J9" s="80" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10">
@@ -4006,24 +4344,24 @@
         <v>45693.0</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D10" s="81"/>
       <c r="E10" s="81"/>
       <c r="F10" s="35" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G10" s="33" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H10" s="82" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I10" s="82" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J10" s="37" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K10" s="84"/>
     </row>
@@ -4032,28 +4370,28 @@
         <v>45693.0</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F11" s="79" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H11" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I11" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J11" s="80" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12">
@@ -4061,28 +4399,28 @@
         <v>45693.0</v>
       </c>
       <c r="C12" s="81" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E12" s="33" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F12" s="35" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G12" s="81" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H12" s="82" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I12" s="82" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J12" s="83" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13">
@@ -4090,31 +4428,31 @@
         <v>45691.0</v>
       </c>
       <c r="C13" s="85" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F13" s="40" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G13" s="85" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H13" s="86" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I13" s="86" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J13" s="87" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25">
@@ -4187,36 +4525,36 @@
     </row>
     <row r="2">
       <c r="C2" s="88" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="76" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C4" s="77" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F4" s="77" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G4" s="77" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H4" s="77" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I4" s="77" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J4" s="78" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
@@ -4224,24 +4562,24 @@
         <v>45691.0</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="79" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H5" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I5" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J5" s="80" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6">
@@ -4249,19 +4587,19 @@
         <v>45691.0</v>
       </c>
       <c r="C6" s="81" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F6" s="82" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G6" s="81" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H6" s="71">
         <v>45691.0</v>
@@ -4270,7 +4608,7 @@
         <v>0.0</v>
       </c>
       <c r="J6" s="83" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7">
@@ -4278,19 +4616,19 @@
         <v>45691.0</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F7" s="79" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H7" s="23">
         <v>45721.0</v>
@@ -4299,7 +4637,7 @@
         <v>1.0</v>
       </c>
       <c r="J7" s="80" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8">
@@ -4307,19 +4645,19 @@
         <v>45691.0</v>
       </c>
       <c r="C8" s="81" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E8" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="82" t="s">
-        <v>34</v>
-      </c>
       <c r="G8" s="81" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H8" s="71">
         <v>45751.0</v>
@@ -4328,7 +4666,7 @@
         <v>2.0</v>
       </c>
       <c r="J8" s="83" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9">
@@ -4336,28 +4674,28 @@
         <v>45691.0</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F9" s="79" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H9" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I9" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J9" s="80" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10">
@@ -4365,24 +4703,24 @@
         <v>45693.0</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D10" s="81"/>
       <c r="E10" s="81"/>
       <c r="F10" s="35" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G10" s="33" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H10" s="82" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I10" s="82" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J10" s="37" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K10" s="84"/>
     </row>
@@ -4391,31 +4729,31 @@
         <v>45691.0</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H11" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I11" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J11" s="80" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12">
@@ -4423,28 +4761,28 @@
         <v>45693.0</v>
       </c>
       <c r="C12" s="81" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E12" s="33" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F12" s="35" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G12" s="81" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H12" s="82" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I12" s="82" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J12" s="83" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13">
@@ -4452,28 +4790,28 @@
         <v>45693.0</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H13" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I13" s="79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J13" s="80" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14">
@@ -4481,28 +4819,28 @@
         <v>45721.0</v>
       </c>
       <c r="C14" s="81" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="33" t="s">
-        <v>35</v>
-      </c>
       <c r="F14" s="35" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G14" s="81" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H14" s="82" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I14" s="82" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J14" s="83" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15">
@@ -4510,28 +4848,28 @@
         <v>45751.0</v>
       </c>
       <c r="C15" s="90" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D15" s="91" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F15" s="92" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G15" s="93" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H15" s="94" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I15" s="94" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J15" s="95" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K15" s="96"/>
     </row>

</xml_diff>